<commit_message>
E-File Import Test class Optimisation done
</commit_message>
<xml_diff>
--- a/data/BppTrend/Valid_Import_Files/BOE Valuation Factors 2021.xlsx
+++ b/data/BppTrend/Valid_Import_Files/BOE Valuation Factors 2021.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deedeepi1\Documents\Sikander's BPP Files\BppTrend\BppTrend\Valid_Import_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deedeepi1\Automation\apasnew\qa_automation\data\BppTrend\Valid_Import_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Document Details" sheetId="12" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Tabs</t>
   </si>
@@ -128,12 +128,6 @@
   </si>
   <si>
     <t>Schedule B - Fixture</t>
-  </si>
-  <si>
-    <t>Junk_A</t>
-  </si>
-  <si>
-    <t>Junk_B</t>
   </si>
 </sst>
 </file>
@@ -240,7 +234,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -332,7 +326,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -737,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -767,8 +760,8 @@
       <c r="B2">
         <v>54</v>
       </c>
-      <c r="C2" t="s">
-        <v>30</v>
+      <c r="C2">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -778,8 +771,8 @@
       <c r="B3">
         <v>54</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>31</v>
+      <c r="C3">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -909,8 +902,8 @@
       <c r="B2" s="24">
         <v>78</v>
       </c>
-      <c r="C2" t="s">
-        <v>30</v>
+      <c r="C2" s="30">
+        <v>77</v>
       </c>
       <c r="D2" s="12"/>
     </row>
@@ -921,8 +914,8 @@
       <c r="B3" s="24">
         <v>78</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>31</v>
+      <c r="C3" s="30">
+        <v>67</v>
       </c>
       <c r="D3" s="12"/>
     </row>
@@ -1235,8 +1228,8 @@
       <c r="C2" s="25">
         <v>92</v>
       </c>
-      <c r="D2" t="s">
-        <v>30</v>
+      <c r="D2" s="25">
+        <v>92</v>
       </c>
       <c r="E2" s="25">
         <v>92</v>
@@ -1252,8 +1245,8 @@
       <c r="C3" s="25">
         <v>92</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>31</v>
+      <c r="D3" s="26">
+        <v>85</v>
       </c>
       <c r="E3" s="25">
         <v>92</v>
@@ -1477,30 +1470,30 @@
     </row>
     <row r="24" spans="1:5" ht="15.75">
       <c r="A24" s="7"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5" ht="15.75">
       <c r="A25" s="8"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="20"/>
     </row>
     <row r="26" spans="1:5" ht="15">
       <c r="A26" s="8"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5" ht="15">
       <c r="A27" s="9"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
       <c r="E27" s="19"/>
     </row>
     <row r="28" spans="1:5" ht="15">
@@ -1773,16 +1766,16 @@
       <c r="A2" s="22">
         <v>2020</v>
       </c>
-      <c r="B2" t="s">
-        <v>30</v>
+      <c r="B2">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="22">
         <v>2019</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>31</v>
+      <c r="B3">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1874,8 +1867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1896,16 +1889,16 @@
       <c r="A2" s="2">
         <v>2020</v>
       </c>
-      <c r="B2" t="s">
-        <v>30</v>
+      <c r="B2">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2019</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>31</v>
+      <c r="B3">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2018,21 +2011,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DC045639EA034996508D08AC8F77A4" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7dbf7a819558f3aedc25624ce3a3d643">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="928b0ed4-59de-4866-ab39-c285c276cabe" xmlns:ns3="10427840-475b-49c9-8fdb-b62ed56f40ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="999177114d252612893f88a2cdbefd84" ns2:_="" ns3:_="">
     <xsd:import namespace="928b0ed4-59de-4866-ab39-c285c276cabe"/>
@@ -2249,24 +2227,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3042FB5-FB08-4B9F-9044-0268488FBE5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EFFB5BE-0098-48C2-BBB0-46C3FEF9D505}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{776E15DF-FD92-4098-830A-BCD94A53755E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2283,4 +2259,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EFFB5BE-0098-48C2-BBB0-46C3FEF9D505}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3042FB5-FB08-4B9F-9044-0268488FBE5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>